<commit_message>
Use clock package for rounding down dates.
</commit_message>
<xml_diff>
--- a/data-raw/cgm_names_labels.xlsx
+++ b/data-raw/cgm_names_labels.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{656686AD-DFEB-4DCF-AA52-5481676E228F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7A370-93A6-4EB9-8557-58E96B8F8DC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B7A370-93A6-4EB9-8557-58E96B8F8DC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -651,7 +651,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>